<commit_message>
- BUG: Main canvas was not getting updated when new dataset was being loaded on top of old one. - CHG: Button that allows viewing of all labels was disabled at low zoom level. This is not helpful when users have a low density map and they want to see it all at a glance. Have re-enabled button for all zoom levels and it is now up to the user to decide whether they want to see all labels or not. - CHG: Actions for find features and find features in range now clear the canvas first. - BUG: Fixed several bugs to do with proper display of canvas and labels after around feature find/range exploration. - BUG: Fixed bug in number formatted parsing of range find dialog.
</commit_message>
<xml_diff>
--- a/data/singleLineFileFormatExample.xlsx
+++ b/data/singleLineFileFormatExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>[this line is not part of the file format itself]</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://penguin.scri.ac.uk/paul/germinate/germinate_development/app/flapjack/flapjack_search/search.pl?marker=</t>
+  </si>
+  <si>
+    <t>http://rice.plantbiology.msu.edu/cgi-bin/gbrowse/rice/?name=</t>
   </si>
 </sst>
 </file>
@@ -452,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -657,6 +666,42 @@
       </c>
       <c r="G8" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1">
+      <c r="A9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- NEW: Have enabled unlimited number of genomes to be loaded. This means that we can now even load the same dataset in twice, albeit under a different name.
</commit_message>
<xml_diff>
--- a/data/singleLineFileFormatExample.xlsx
+++ b/data/singleLineFileFormatExample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="2130" windowWidth="23085" windowHeight="4710"/>
+    <workbookView xWindow="19185" yWindow="-15" windowWidth="9660" windowHeight="13815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>type</t>
   </si>
@@ -99,15 +99,9 @@
     <t>LOC_Os05g01020</t>
   </si>
   <si>
-    <t>protein paired amphipathic helix repeat family protein, expressed</t>
-  </si>
-  <si>
     <t>LOC_Os09g20010</t>
   </si>
   <si>
-    <t>protein SNF1-related protein kinase regulatory subunit beta-2, putative, expressed</t>
-  </si>
-  <si>
     <t>[this line is not part of the file format itself]</t>
   </si>
   <si>
@@ -118,6 +112,9 @@
   </si>
   <si>
     <t>http://rice.plantbiology.msu.edu/cgi-bin/gbrowse/rice/?name=</t>
+  </si>
+  <si>
+    <t>any comment here</t>
   </si>
 </sst>
 </file>
@@ -464,7 +461,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,7 +498,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -619,7 +616,7 @@
         <v>6</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -642,7 +639,7 @@
         <v>6.9999999999999997E-91</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -659,13 +656,13 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F8" s="1">
         <v>5.9999999999999998E-50</v>
       </c>
       <c r="G8" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1">
@@ -676,32 +673,32 @@
         <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- CHG: Deleted redundant classes DataImporter, GFeature and GLink. - CHG: Renamed the main class to Strudel.java and the example file to have a .strudel extension. - NEW: Added feature type field to single file data format.
</commit_message>
<xml_diff>
--- a/data/singleLineFileFormatExample.xlsx
+++ b/data/singleLineFileFormatExample.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>type</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>any comment here</t>
+  </si>
+  <si>
+    <t>featureType</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>SNP</t>
   </si>
 </sst>
 </file>
@@ -458,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,13 +478,15 @@
     <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="76.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="76.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="53" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1">
+    <row r="1" spans="1:9" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -489,19 +500,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -514,17 +528,20 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="E2">
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2">
         <v>1903</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -537,17 +554,20 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3">
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3">
         <v>10218</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -560,17 +580,20 @@
       <c r="D4" t="s">
         <v>16</v>
       </c>
-      <c r="E4">
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4">
         <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -583,17 +606,20 @@
       <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5">
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5">
         <v>0.75</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" s="2" customFormat="1">
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
@@ -619,7 +645,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -642,7 +668,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -665,7 +691,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1">
+    <row r="9" spans="1:9" s="2" customFormat="1">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -675,11 +701,11 @@
       <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -690,7 +716,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>29</v>
       </c>

</xml_diff>